<commit_message>
Round 3 final setup
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Round 3/Advanced.xlsx
+++ b/public/res/leaderboards/Round 3/Advanced.xlsx
@@ -1,188 +1,175 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzaqureshi/Documents/Programming/Python/poker-tournament-leaderboard/public/res/leaderboards/Round 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzaqureshi/Documents/Programming/Python/QTS/add_new_players/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69251ED9-8DC2-674A-BE5A-F0DEB6CF807D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC19B6F-7E9C-EF43-B052-116518379467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700"/>
   </bookViews>
   <sheets>
     <sheet name="Advanced" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Ethan Lim</t>
+  </si>
+  <si>
+    <t>Richard Shao</t>
+  </si>
+  <si>
+    <t>Ethan Yuen</t>
+  </si>
+  <si>
+    <t>Oliver He</t>
+  </si>
+  <si>
+    <t>Thomas Ross</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qianglin </t>
+  </si>
+  <si>
+    <t>Yalun Yang</t>
+  </si>
+  <si>
+    <t>Alan Qiu</t>
+  </si>
+  <si>
+    <t>Chia lester</t>
+  </si>
+  <si>
+    <t>Grant Fullston</t>
+  </si>
+  <si>
+    <t>Jules Seng</t>
+  </si>
+  <si>
+    <t>Nicolas Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guan Zhen Gan </t>
+  </si>
+  <si>
+    <t>CHAK SAN WU</t>
+  </si>
+  <si>
+    <t>WENG HIN CHOI</t>
+  </si>
+  <si>
+    <t>Yuwei Zhao</t>
+  </si>
+  <si>
+    <t>Abhishek Tummalapalli</t>
+  </si>
+  <si>
+    <t>Hamza Qureshi</t>
+  </si>
+  <si>
+    <t>Lai Shun Cheong</t>
+  </si>
+  <si>
+    <t>William Cheung</t>
+  </si>
+  <si>
+    <t>Luca Piffaretti</t>
+  </si>
+  <si>
+    <t>Matt Cho</t>
+  </si>
+  <si>
+    <t>Lingze Xu</t>
+  </si>
+  <si>
+    <t>Mody Yim</t>
+  </si>
+  <si>
+    <t>Isak W√§rnman</t>
+  </si>
+  <si>
+    <t>Bevan Lovejoy</t>
+  </si>
+  <si>
+    <t>Patrick Grave</t>
+  </si>
+  <si>
+    <t>Anton Huynh</t>
+  </si>
+  <si>
+    <t>Connor Gundberg</t>
+  </si>
+  <si>
+    <t>Alix Zhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runqiu Fei </t>
+  </si>
+  <si>
+    <t>Shengjie Yu</t>
+  </si>
+  <si>
+    <t>James Dainton</t>
+  </si>
+  <si>
+    <t>Kayson Wang</t>
+  </si>
+  <si>
+    <t>Li Wong</t>
+  </si>
+  <si>
+    <t>Choi Chon Lok</t>
+  </si>
+  <si>
+    <t>Zixuan Huang</t>
+  </si>
+  <si>
+    <t>Zichao Sang</t>
+  </si>
+  <si>
+    <t>Saaiq Ahmed</t>
+  </si>
+  <si>
+    <t>Simon Creaner</t>
+  </si>
+  <si>
+    <t>Daniel li</t>
+  </si>
+  <si>
+    <t>Even Guo</t>
+  </si>
+  <si>
+    <t>James Tyrikos</t>
+  </si>
+  <si>
     <t>#</t>
   </si>
   <si>
-    <t>Round 1</t>
-  </si>
-  <si>
-    <t>Round 2</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Ethan Lim</t>
-  </si>
-  <si>
-    <t>Richard Shao</t>
-  </si>
-  <si>
-    <t>Ethan Yuen</t>
-  </si>
-  <si>
-    <t>Oliver He</t>
-  </si>
-  <si>
-    <t>Thomas Ross</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qianglin </t>
-  </si>
-  <si>
-    <t>Yalun Yang</t>
-  </si>
-  <si>
-    <t>Alan Qiu</t>
-  </si>
-  <si>
-    <t>Grant Fullston</t>
-  </si>
-  <si>
-    <t>Jules Seng</t>
-  </si>
-  <si>
-    <t>Nicolas Garcia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guan Zhen Gan </t>
-  </si>
-  <si>
-    <t>CHAK SAN WU</t>
-  </si>
-  <si>
-    <t>WENG HIN CHOI</t>
-  </si>
-  <si>
-    <t>Yuwei Zhao</t>
-  </si>
-  <si>
-    <t>Abhishek Tummalapalli</t>
-  </si>
-  <si>
-    <t>Hamza Qureshi</t>
-  </si>
-  <si>
-    <t>Lai Shun Cheong</t>
-  </si>
-  <si>
-    <t>William Cheung</t>
-  </si>
-  <si>
-    <t>Luca Piffaretti</t>
-  </si>
-  <si>
-    <t>Matt Cho</t>
-  </si>
-  <si>
-    <t>Lingze Xu</t>
-  </si>
-  <si>
-    <t>Mody Yim</t>
-  </si>
-  <si>
-    <t>Isak W√§rnman</t>
-  </si>
-  <si>
-    <t>Bevan Lovejoy</t>
-  </si>
-  <si>
-    <t>Patrick Grave</t>
-  </si>
-  <si>
-    <t>Anton Huynh</t>
-  </si>
-  <si>
-    <t>Connor Gundberg</t>
-  </si>
-  <si>
-    <t>Alix Zhu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runqiu Fei </t>
-  </si>
-  <si>
-    <t>Shengjie Yu</t>
-  </si>
-  <si>
-    <t>James Dainton</t>
-  </si>
-  <si>
-    <t>Kayson Wang</t>
-  </si>
-  <si>
-    <t>Li Wong</t>
-  </si>
-  <si>
-    <t>Choi Chon Lok</t>
-  </si>
-  <si>
-    <t>Zixuan Huang</t>
-  </si>
-  <si>
-    <t>Zichao Sang</t>
-  </si>
-  <si>
-    <t>Saaiq Ahmed</t>
-  </si>
-  <si>
-    <t>Simon Creaner</t>
-  </si>
-  <si>
-    <t>Daniel li</t>
-  </si>
-  <si>
-    <t>Even Guo</t>
-  </si>
-  <si>
-    <t>James Tyrikos</t>
-  </si>
-  <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Chia Lester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1016,30 +1003,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="A2" sqref="A2:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1047,13 +1034,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>114400</v>
+        <v>84400</v>
       </c>
       <c r="D2">
-        <v>107500</v>
+        <v>77500</v>
       </c>
       <c r="E2">
         <v>161900</v>
@@ -1064,13 +1051,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>76400</v>
+        <v>46400</v>
       </c>
       <c r="D3">
-        <v>76400</v>
+        <v>68100</v>
       </c>
       <c r="E3">
         <v>114500</v>
@@ -1081,13 +1068,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>155000</v>
+        <v>125000</v>
       </c>
       <c r="D4">
-        <v>155000</v>
+        <v>-30000</v>
       </c>
       <c r="E4">
         <v>95000</v>
@@ -1098,13 +1085,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>140000</v>
+        <v>110000</v>
       </c>
       <c r="D5">
-        <v>140000</v>
+        <v>-30000</v>
       </c>
       <c r="E5">
         <v>80000</v>
@@ -1115,13 +1102,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>36600</v>
+        <v>6600</v>
       </c>
       <c r="D6">
-        <v>36600</v>
+        <v>62100</v>
       </c>
       <c r="E6">
         <v>68700</v>
@@ -1132,13 +1119,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>123200</v>
+        <v>93200</v>
       </c>
       <c r="D7">
-        <v>123200</v>
+        <v>-30000</v>
       </c>
       <c r="E7">
         <v>63200</v>
@@ -1149,13 +1136,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>-30000</v>
       </c>
       <c r="D8">
-        <v>-30000</v>
+        <v>92000</v>
       </c>
       <c r="E8">
         <v>62000</v>
@@ -1166,13 +1153,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>120800</v>
+        <v>90800</v>
       </c>
       <c r="D9">
-        <v>120800</v>
+        <v>-30000</v>
       </c>
       <c r="E9">
         <v>60800</v>
@@ -1183,13 +1170,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>94500</v>
+        <v>64500</v>
       </c>
       <c r="D10">
-        <v>94500</v>
+        <v>-25000</v>
       </c>
       <c r="E10">
         <v>39500</v>
@@ -1203,10 +1190,10 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>84600</v>
+        <v>54600</v>
       </c>
       <c r="D11">
-        <v>84600</v>
+        <v>-30000</v>
       </c>
       <c r="E11">
         <v>24600</v>
@@ -1220,10 +1207,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>44800</v>
+        <v>14800</v>
       </c>
       <c r="D12">
-        <v>44800</v>
+        <v>6200</v>
       </c>
       <c r="E12">
         <v>21000</v>
@@ -1237,10 +1224,10 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>74600</v>
+        <v>44600</v>
       </c>
       <c r="D13">
-        <v>74600</v>
+        <v>-30000</v>
       </c>
       <c r="E13">
         <v>14600</v>
@@ -1257,7 +1244,7 @@
         <v>-30000</v>
       </c>
       <c r="D14">
-        <v>-30000</v>
+        <v>44000</v>
       </c>
       <c r="E14">
         <v>14000</v>
@@ -1271,10 +1258,10 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>37000</v>
+        <v>7000</v>
       </c>
       <c r="D15">
-        <v>37000</v>
+        <v>4000</v>
       </c>
       <c r="E15">
         <v>11000</v>
@@ -1288,10 +1275,10 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>30400</v>
+        <v>400</v>
       </c>
       <c r="D16">
-        <v>30400</v>
+        <v>4000</v>
       </c>
       <c r="E16">
         <v>4400</v>
@@ -1305,10 +1292,10 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>17100</v>
+        <v>-12900</v>
       </c>
       <c r="D17">
-        <v>17100</v>
+        <v>14900</v>
       </c>
       <c r="E17">
         <v>2000</v>
@@ -1325,7 +1312,7 @@
         <v>-30000</v>
       </c>
       <c r="D18">
-        <v>-30000</v>
+        <v>28800</v>
       </c>
       <c r="E18">
         <v>-1200</v>
@@ -1342,7 +1329,7 @@
         <v>-30000</v>
       </c>
       <c r="D19">
-        <v>-30000</v>
+        <v>28000</v>
       </c>
       <c r="E19">
         <v>-2000</v>
@@ -1359,7 +1346,7 @@
         <v>-30000</v>
       </c>
       <c r="D20">
-        <v>-30000</v>
+        <v>23900</v>
       </c>
       <c r="E20">
         <v>-6100</v>
@@ -1376,7 +1363,7 @@
         <v>-30000</v>
       </c>
       <c r="D21">
-        <v>-30000</v>
+        <v>17700</v>
       </c>
       <c r="E21">
         <v>-12300</v>
@@ -1390,10 +1377,10 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>32400</v>
+        <v>2400</v>
       </c>
       <c r="D22">
-        <v>32400</v>
+        <v>-30000</v>
       </c>
       <c r="E22">
         <v>-27600</v>
@@ -1407,10 +1394,10 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>24600</v>
+        <v>-5400</v>
       </c>
       <c r="D23">
-        <v>24600</v>
+        <v>-30000</v>
       </c>
       <c r="E23">
         <v>-35400</v>
@@ -1424,10 +1411,10 @@
         <v>25</v>
       </c>
       <c r="C24">
-        <v>19800</v>
+        <v>-10200</v>
       </c>
       <c r="D24">
-        <v>19800</v>
+        <v>-30000</v>
       </c>
       <c r="E24">
         <v>-40200</v>
@@ -1441,10 +1428,10 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>13200</v>
+        <v>-16800</v>
       </c>
       <c r="D25">
-        <v>13200</v>
+        <v>-30000</v>
       </c>
       <c r="E25">
         <v>-46800</v>
@@ -1730,10 +1717,10 @@
         <v>43</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>-30000</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>-30000</v>
       </c>
       <c r="E42">
         <v>-60000</v>

</xml_diff>